<commit_message>
added data for dec
</commit_message>
<xml_diff>
--- a/Inputs/InputSchedule2.xlsx
+++ b/Inputs/InputSchedule2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ah17992_bristol_ac_uk/Documents/DP5/Shared/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{367989ED-20DD-419D-812E-58AFD0589065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E8ED544-55E2-466C-A005-CB500FA81848}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="13_ncr:1_{367989ED-20DD-419D-812E-58AFD0589065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{538AE27F-DA60-4C90-8DFE-E7BF57A83F22}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="109">
   <si>
     <t>Case</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>ICE</t>
+  </si>
+  <si>
+    <t>Dec House Charging</t>
   </si>
 </sst>
 </file>
@@ -926,7 +929,161 @@
     <cellStyle name="Total" xfId="40" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="41" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="169">
+  <dxfs count="188">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2627,10 +2784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BR109"/>
+  <dimension ref="A1:BR120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AO98" sqref="AO98"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23314,851 +23471,3025 @@
         <v>50</v>
       </c>
     </row>
+    <row r="110" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A110" s="8">
+        <v>1</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C110" t="s">
+        <v>108</v>
+      </c>
+      <c r="E110" s="8">
+        <v>0</v>
+      </c>
+      <c r="F110" s="9"/>
+      <c r="G110" s="8">
+        <v>54</v>
+      </c>
+      <c r="H110" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I110" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J110" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K110" s="8">
+        <v>1</v>
+      </c>
+      <c r="L110" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M110" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N110" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O110" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P110" s="10"/>
+      <c r="Q110" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R110" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S110" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T110" s="8">
+        <v>4</v>
+      </c>
+      <c r="U110" s="8">
+        <v>1</v>
+      </c>
+      <c r="W110" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X110" s="13">
+        <v>44536</v>
+      </c>
+      <c r="Y110" s="13">
+        <v>44543</v>
+      </c>
+      <c r="Z110" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA110" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB110" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC110" s="13">
+        <v>44543</v>
+      </c>
+      <c r="AE110" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF110" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG110" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI110" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ110" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK110" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL110">
+        <v>1</v>
+      </c>
+      <c r="AN110" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO110" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP110" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ110" s="10"/>
+      <c r="AR110" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS110" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT110" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU110" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV110" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW110" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX110" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY110" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ110" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA110" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB110" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC110" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD110" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE110" s="10"/>
+      <c r="BF110" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG110" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH110" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI110" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ110" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK110" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL110" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM110" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN110" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO110" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP110" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ110" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR110" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A111" s="8">
+        <v>1</v>
+      </c>
+      <c r="B111" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C111" t="s">
+        <v>82</v>
+      </c>
+      <c r="E111" s="8">
+        <v>0</v>
+      </c>
+      <c r="F111" s="9"/>
+      <c r="G111" s="8">
+        <v>54</v>
+      </c>
+      <c r="H111" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I111" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J111" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K111" s="8">
+        <v>1</v>
+      </c>
+      <c r="L111" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M111" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N111" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O111" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P111" s="10"/>
+      <c r="Q111" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R111" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S111" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T111" s="8">
+        <v>4</v>
+      </c>
+      <c r="U111" s="8">
+        <v>1</v>
+      </c>
+      <c r="W111" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X111" s="13">
+        <v>44535.791666666664</v>
+      </c>
+      <c r="Y111" s="13">
+        <v>44536.354166666664</v>
+      </c>
+      <c r="Z111" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA111" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB111" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC111" s="13">
+        <v>44536.354166666664</v>
+      </c>
+      <c r="AE111" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF111" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG111" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI111" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ111" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK111" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL111">
+        <v>0</v>
+      </c>
+      <c r="AN111" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO111" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP111" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ111" s="10"/>
+      <c r="AR111" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS111" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT111" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU111" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV111" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW111" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX111" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY111" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ111" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA111" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB111" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC111" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD111" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE111" s="10"/>
+      <c r="BF111" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG111" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH111" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI111" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ111" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK111" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL111" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM111" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN111" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO111" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP111" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ111" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR111" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A112" s="8">
+        <v>1</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C112" t="s">
+        <v>77</v>
+      </c>
+      <c r="E112" s="8">
+        <v>0</v>
+      </c>
+      <c r="F112" s="9"/>
+      <c r="G112" s="8">
+        <v>54</v>
+      </c>
+      <c r="H112" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I112" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J112" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K112" s="8">
+        <v>1</v>
+      </c>
+      <c r="L112" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M112" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N112" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O112" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P112" s="10"/>
+      <c r="Q112" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R112" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S112" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T112" s="8">
+        <v>4</v>
+      </c>
+      <c r="U112" s="8">
+        <v>1</v>
+      </c>
+      <c r="W112" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X112" s="13">
+        <v>44536.770833333336</v>
+      </c>
+      <c r="Y112" s="13">
+        <v>44536.8125</v>
+      </c>
+      <c r="Z112" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA112" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB112" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC112" s="13">
+        <v>44536.8125</v>
+      </c>
+      <c r="AE112" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF112" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG112" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI112" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ112" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK112" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL112">
+        <v>0</v>
+      </c>
+      <c r="AN112" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO112" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP112" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ112" s="10"/>
+      <c r="AR112" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS112" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT112" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU112" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV112" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW112" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX112" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY112" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ112" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA112" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB112" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC112" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD112" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE112" s="10"/>
+      <c r="BF112" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG112" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH112" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI112" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ112" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK112" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL112" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM112" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN112" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO112" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP112" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ112" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR112" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A113" s="8">
+        <v>1</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C113" t="s">
+        <v>81</v>
+      </c>
+      <c r="E113" s="8">
+        <v>0</v>
+      </c>
+      <c r="F113" s="9"/>
+      <c r="G113" s="8">
+        <v>54</v>
+      </c>
+      <c r="H113" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I113" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J113" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K113" s="8">
+        <v>1</v>
+      </c>
+      <c r="L113" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M113" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N113" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O113" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P113" s="10"/>
+      <c r="Q113" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R113" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S113" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T113" s="8">
+        <v>4</v>
+      </c>
+      <c r="U113" s="8">
+        <v>1</v>
+      </c>
+      <c r="W113" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X113" s="13">
+        <v>44536.854166666664</v>
+      </c>
+      <c r="Y113" s="13">
+        <v>44537.354166666664</v>
+      </c>
+      <c r="Z113" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA113" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB113" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC113" s="13">
+        <v>44537.354166666664</v>
+      </c>
+      <c r="AE113" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF113" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG113" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI113" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ113" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK113" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL113">
+        <v>0</v>
+      </c>
+      <c r="AN113" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO113" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP113" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ113" s="10"/>
+      <c r="AR113" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS113" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT113" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU113" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV113" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW113" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX113" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY113" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ113" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA113" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB113" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC113" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD113" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE113" s="10"/>
+      <c r="BF113" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG113" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH113" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI113" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ113" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK113" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL113" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM113" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN113" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO113" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP113" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ113" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR113" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A114" s="8">
+        <v>1</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C114" t="s">
+        <v>80</v>
+      </c>
+      <c r="E114" s="8">
+        <v>0</v>
+      </c>
+      <c r="F114" s="9"/>
+      <c r="G114" s="8">
+        <v>54</v>
+      </c>
+      <c r="H114" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I114" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J114" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K114" s="8">
+        <v>1</v>
+      </c>
+      <c r="L114" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M114" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N114" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O114" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P114" s="10"/>
+      <c r="Q114" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R114" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S114" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T114" s="8">
+        <v>4</v>
+      </c>
+      <c r="U114" s="8">
+        <v>1</v>
+      </c>
+      <c r="W114" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X114" s="13">
+        <v>44537.770833333336</v>
+      </c>
+      <c r="Y114" s="13">
+        <v>44538.354166666664</v>
+      </c>
+      <c r="Z114" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA114" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB114" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC114" s="13">
+        <v>44538.354166666664</v>
+      </c>
+      <c r="AE114" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF114" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG114" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI114" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ114" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK114" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL114">
+        <v>0</v>
+      </c>
+      <c r="AN114" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO114" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP114" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ114" s="10"/>
+      <c r="AR114" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS114" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT114" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU114" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV114" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW114" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX114" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY114" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ114" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA114" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB114" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC114" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD114" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE114" s="10"/>
+      <c r="BF114" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG114" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH114" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI114" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ114" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK114" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL114" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM114" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN114" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO114" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP114" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ114" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR114" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A115" s="8">
+        <v>1</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C115" t="s">
+        <v>78</v>
+      </c>
+      <c r="E115" s="8">
+        <v>0</v>
+      </c>
+      <c r="F115" s="9"/>
+      <c r="G115" s="8">
+        <v>54</v>
+      </c>
+      <c r="H115" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I115" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J115" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K115" s="8">
+        <v>1</v>
+      </c>
+      <c r="L115" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M115" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N115" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O115" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P115" s="10"/>
+      <c r="Q115" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R115" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S115" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T115" s="8">
+        <v>4</v>
+      </c>
+      <c r="U115" s="8">
+        <v>1</v>
+      </c>
+      <c r="W115" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X115" s="13">
+        <v>44538.770833333336</v>
+      </c>
+      <c r="Y115" s="13">
+        <v>44538.8125</v>
+      </c>
+      <c r="Z115" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA115" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB115" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC115" s="13">
+        <v>44538.8125</v>
+      </c>
+      <c r="AE115" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF115" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG115" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI115" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ115" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK115" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL115">
+        <v>0</v>
+      </c>
+      <c r="AN115" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO115" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP115" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ115" s="10"/>
+      <c r="AR115" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS115" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT115" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU115" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV115" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW115" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX115" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY115" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ115" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA115" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB115" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC115" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD115" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE115" s="10"/>
+      <c r="BF115" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG115" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH115" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI115" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ115" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK115" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL115" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM115" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN115" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO115" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP115" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ115" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR115" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="116" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A116" s="8">
+        <v>1</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C116" t="s">
+        <v>79</v>
+      </c>
+      <c r="E116" s="8">
+        <v>0</v>
+      </c>
+      <c r="F116" s="9"/>
+      <c r="G116" s="8">
+        <v>54</v>
+      </c>
+      <c r="H116" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I116" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J116" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K116" s="8">
+        <v>1</v>
+      </c>
+      <c r="L116" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M116" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N116" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O116" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R116" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S116" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T116" s="8">
+        <v>4</v>
+      </c>
+      <c r="U116" s="8">
+        <v>1</v>
+      </c>
+      <c r="W116" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X116" s="13">
+        <v>44538.854166666664</v>
+      </c>
+      <c r="Y116" s="13">
+        <v>44539.354166666664</v>
+      </c>
+      <c r="Z116" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA116" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB116" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC116" s="13">
+        <v>44539.354166666664</v>
+      </c>
+      <c r="AE116" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF116" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG116" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI116" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ116" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK116" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL116">
+        <v>0</v>
+      </c>
+      <c r="AN116" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO116" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP116" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ116" s="10"/>
+      <c r="AR116" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS116" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT116" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU116" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV116" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW116" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX116" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY116" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ116" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA116" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB116" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC116" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD116" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE116" s="10"/>
+      <c r="BF116" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG116" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH116" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI116" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ116" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK116" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL116" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM116" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN116" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO116" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP116" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ116" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR116" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="117" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A117" s="8">
+        <v>1</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C117" t="s">
+        <v>83</v>
+      </c>
+      <c r="E117" s="8">
+        <v>0</v>
+      </c>
+      <c r="F117" s="9"/>
+      <c r="G117" s="8">
+        <v>54</v>
+      </c>
+      <c r="H117" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I117" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J117" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K117" s="8">
+        <v>1</v>
+      </c>
+      <c r="L117" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M117" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N117" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O117" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P117" s="10"/>
+      <c r="Q117" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R117" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S117" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T117" s="8">
+        <v>4</v>
+      </c>
+      <c r="U117" s="8">
+        <v>1</v>
+      </c>
+      <c r="W117" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X117" s="13">
+        <v>44539.770833333336</v>
+      </c>
+      <c r="Y117" s="13">
+        <v>44540.354166666664</v>
+      </c>
+      <c r="Z117" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA117" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB117" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC117" s="13">
+        <v>44540.354166666664</v>
+      </c>
+      <c r="AE117" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF117" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG117" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI117" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ117" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK117" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL117">
+        <v>0</v>
+      </c>
+      <c r="AN117" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO117" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP117" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ117" s="10"/>
+      <c r="AR117" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS117" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT117" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU117" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV117" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW117" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX117" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY117" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ117" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA117" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB117" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC117" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD117" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE117" s="10"/>
+      <c r="BF117" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG117" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH117" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI117" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ117" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK117" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL117" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM117" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN117" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO117" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP117" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ117" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR117" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A118" s="8">
+        <v>1</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C118" t="s">
+        <v>84</v>
+      </c>
+      <c r="E118" s="8">
+        <v>0</v>
+      </c>
+      <c r="F118" s="9"/>
+      <c r="G118" s="8">
+        <v>54</v>
+      </c>
+      <c r="H118" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I118" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J118" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K118" s="8">
+        <v>1</v>
+      </c>
+      <c r="L118" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M118" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N118" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O118" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R118" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S118" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T118" s="8">
+        <v>4</v>
+      </c>
+      <c r="U118" s="8">
+        <v>1</v>
+      </c>
+      <c r="W118" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X118" s="13">
+        <v>44540.770833333336</v>
+      </c>
+      <c r="Y118" s="13">
+        <v>44540.8125</v>
+      </c>
+      <c r="Z118" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA118" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB118" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC118" s="13">
+        <v>44540.8125</v>
+      </c>
+      <c r="AE118" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF118" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG118" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI118" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ118" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK118" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL118">
+        <v>0</v>
+      </c>
+      <c r="AN118" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO118" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP118" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ118" s="10"/>
+      <c r="AR118" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS118" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT118" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU118" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV118" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW118" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX118" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY118" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ118" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA118" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB118" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC118" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD118" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE118" s="10"/>
+      <c r="BF118" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG118" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH118" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI118" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ118" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK118" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL118" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM118" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN118" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO118" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP118" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ118" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR118" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="119" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A119" s="8">
+        <v>1</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C119" t="s">
+        <v>85</v>
+      </c>
+      <c r="E119" s="8">
+        <v>0</v>
+      </c>
+      <c r="F119" s="9"/>
+      <c r="G119" s="8">
+        <v>54</v>
+      </c>
+      <c r="H119" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I119" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J119" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K119" s="8">
+        <v>1</v>
+      </c>
+      <c r="L119" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M119" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N119" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O119" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P119" s="10"/>
+      <c r="Q119" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R119" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S119" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T119" s="8">
+        <v>4</v>
+      </c>
+      <c r="U119" s="8">
+        <v>1</v>
+      </c>
+      <c r="W119" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X119" s="13">
+        <v>44540.854166666664</v>
+      </c>
+      <c r="Y119" s="13">
+        <v>44541.354166666664</v>
+      </c>
+      <c r="Z119" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA119" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB119" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC119" s="13">
+        <v>44541.354166666664</v>
+      </c>
+      <c r="AE119" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF119" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG119" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI119" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ119" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK119" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL119">
+        <v>0</v>
+      </c>
+      <c r="AN119" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO119" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP119" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ119" s="10"/>
+      <c r="AR119" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS119" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT119" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU119" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV119" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW119" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX119" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY119" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ119" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA119" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB119" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC119" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD119" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE119" s="10"/>
+      <c r="BF119" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG119" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH119" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI119" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ119" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK119" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL119" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM119" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN119" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO119" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP119" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ119" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR119" s="8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="120" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="A120" s="8">
+        <v>1</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C120" t="s">
+        <v>86</v>
+      </c>
+      <c r="E120" s="8">
+        <v>0</v>
+      </c>
+      <c r="F120" s="9"/>
+      <c r="G120" s="8">
+        <v>54</v>
+      </c>
+      <c r="H120" s="8">
+        <v>59000</v>
+      </c>
+      <c r="I120" s="8">
+        <v>13700</v>
+      </c>
+      <c r="J120" s="8">
+        <v>2437.5</v>
+      </c>
+      <c r="K120" s="8">
+        <v>1</v>
+      </c>
+      <c r="L120" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="M120" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="N120" s="8">
+        <v>7.4</v>
+      </c>
+      <c r="O120" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="P120" s="10"/>
+      <c r="Q120" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="R120" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S120" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T120" s="8">
+        <v>4</v>
+      </c>
+      <c r="U120" s="8">
+        <v>1</v>
+      </c>
+      <c r="W120" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="X120" s="13">
+        <v>44541.770833333336</v>
+      </c>
+      <c r="Y120" s="13">
+        <v>44543</v>
+      </c>
+      <c r="Z120" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA120" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB120" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC120" s="13">
+        <v>44543</v>
+      </c>
+      <c r="AE120" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF120" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG120" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI120" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ120" s="8">
+        <v>9</v>
+      </c>
+      <c r="AK120" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="AL120">
+        <v>0</v>
+      </c>
+      <c r="AN120" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO120" s="8">
+        <v>5</v>
+      </c>
+      <c r="AP120" s="8">
+        <v>6</v>
+      </c>
+      <c r="AQ120" s="10"/>
+      <c r="AR120" s="8">
+        <v>10</v>
+      </c>
+      <c r="AS120" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT120" s="8">
+        <v>10</v>
+      </c>
+      <c r="AU120" s="8">
+        <v>15</v>
+      </c>
+      <c r="AV120" s="8">
+        <v>21</v>
+      </c>
+      <c r="AW120" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AX120" s="8">
+        <v>2000</v>
+      </c>
+      <c r="AY120" s="8">
+        <v>1</v>
+      </c>
+      <c r="AZ120" s="8">
+        <v>40</v>
+      </c>
+      <c r="BA120" s="8">
+        <v>120</v>
+      </c>
+      <c r="BB120" s="8">
+        <v>40</v>
+      </c>
+      <c r="BC120" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="BD120" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="BE120" s="10"/>
+      <c r="BF120" s="8">
+        <v>1</v>
+      </c>
+      <c r="BG120" s="8">
+        <v>355</v>
+      </c>
+      <c r="BH120" s="8">
+        <v>1684</v>
+      </c>
+      <c r="BI120" s="8">
+        <v>1</v>
+      </c>
+      <c r="BJ120" s="8">
+        <v>1</v>
+      </c>
+      <c r="BK120" s="8">
+        <v>1</v>
+      </c>
+      <c r="BL120" s="8">
+        <v>1</v>
+      </c>
+      <c r="BM120" s="8">
+        <v>1</v>
+      </c>
+      <c r="BN120" s="12">
+        <v>46.8</v>
+      </c>
+      <c r="BO120" s="8">
+        <v>143</v>
+      </c>
+      <c r="BP120" s="8">
+        <v>23</v>
+      </c>
+      <c r="BQ120" s="8">
+        <v>150</v>
+      </c>
+      <c r="BR120" s="8">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="Z2:AA21 Y2:Y109">
-    <cfRule type="cellIs" dxfId="168" priority="274" operator="lessThan">
+  <conditionalFormatting sqref="Z2:AA21 Y2:Y120">
+    <cfRule type="cellIs" dxfId="187" priority="293" operator="lessThan">
       <formula>X2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:AA32 Z34:AA43 Z45:AA54 Z100:AA109 Z89:AA98 Z78:AA87 Z67:AA76 Z56:AA65 Z13:AA21 Z4:AA11">
-    <cfRule type="expression" dxfId="167" priority="272" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="291" stopIfTrue="1">
       <formula>Z4&lt;&gt;Z3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ2:BR2 Z2:AA2">
-    <cfRule type="expression" dxfId="166" priority="224" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="243" stopIfTrue="1">
       <formula>Z2&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ3:BR3 Z3:AA3">
-    <cfRule type="expression" dxfId="165" priority="222" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="241" stopIfTrue="1">
       <formula>Z3&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ4:BR4">
-    <cfRule type="expression" dxfId="164" priority="221" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="240" stopIfTrue="1">
       <formula>BQ4&lt;&gt;BQ3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ5:BR11">
-    <cfRule type="expression" dxfId="163" priority="220" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="239" stopIfTrue="1">
       <formula>BQ5&lt;&gt;BQ4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ12:BR12 Z12:AA12">
-    <cfRule type="expression" dxfId="162" priority="219" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="238" stopIfTrue="1">
       <formula>Z12&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ13:BR13">
-    <cfRule type="expression" dxfId="161" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="237" stopIfTrue="1">
       <formula>BQ13&lt;&gt;BQ12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ14:BR14">
-    <cfRule type="expression" dxfId="160" priority="217" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="236" stopIfTrue="1">
       <formula>BQ14&lt;&gt;BQ13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ15:BR15">
-    <cfRule type="expression" dxfId="159" priority="216" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="235" stopIfTrue="1">
       <formula>BQ15&lt;&gt;BQ14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ16:BR21">
-    <cfRule type="expression" dxfId="158" priority="215" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="234" stopIfTrue="1">
       <formula>BQ16&lt;&gt;BQ15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ22:BR22 Z22:AA22 Z33:AA33 Z44:AA44 Z99:AA99 Z88:AA88 Z77:AA77 Z66:AA66 Z55:AA55">
-    <cfRule type="expression" dxfId="157" priority="214" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="233" stopIfTrue="1">
       <formula>Z22&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ23:BR23">
-    <cfRule type="expression" dxfId="156" priority="213" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="232" stopIfTrue="1">
       <formula>BQ23&lt;&gt;BQ22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ24:BR24">
-    <cfRule type="expression" dxfId="155" priority="212" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="231" stopIfTrue="1">
       <formula>BQ24&lt;&gt;BQ23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ25:BR25">
-    <cfRule type="expression" dxfId="154" priority="211" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="230" stopIfTrue="1">
       <formula>BQ25&lt;&gt;BQ24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ26:BR32">
-    <cfRule type="expression" dxfId="153" priority="210" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="229" stopIfTrue="1">
       <formula>BQ26&lt;&gt;BQ25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ33:BR33">
-    <cfRule type="expression" dxfId="152" priority="209" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="228" stopIfTrue="1">
       <formula>BQ33&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ34:BR34">
-    <cfRule type="expression" dxfId="151" priority="208" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="227" stopIfTrue="1">
       <formula>BQ34&lt;&gt;BQ33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ35:BR35">
-    <cfRule type="expression" dxfId="150" priority="207" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="226" stopIfTrue="1">
       <formula>BQ35&lt;&gt;BQ34</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ36:BR36">
-    <cfRule type="expression" dxfId="149" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="225" stopIfTrue="1">
       <formula>BQ36&lt;&gt;BQ35</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ37:BR43">
-    <cfRule type="expression" dxfId="148" priority="205" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="224" stopIfTrue="1">
       <formula>BQ37&lt;&gt;BQ36</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ44:BR44">
-    <cfRule type="expression" dxfId="147" priority="204" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="223" stopIfTrue="1">
       <formula>BQ44&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ45:BR45">
-    <cfRule type="expression" dxfId="146" priority="203" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="222" stopIfTrue="1">
       <formula>BQ45&lt;&gt;BQ44</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ46:BR46">
-    <cfRule type="expression" dxfId="145" priority="202" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="221" stopIfTrue="1">
       <formula>BQ46&lt;&gt;BQ45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ47:BR47">
-    <cfRule type="expression" dxfId="144" priority="201" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="220" stopIfTrue="1">
       <formula>BQ47&lt;&gt;BQ46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ48:BR54">
-    <cfRule type="expression" dxfId="143" priority="200" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="219" stopIfTrue="1">
       <formula>BQ48&lt;&gt;BQ47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ55:BR55">
-    <cfRule type="expression" dxfId="142" priority="199" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="218" stopIfTrue="1">
       <formula>BQ55&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ56:BR56">
-    <cfRule type="expression" dxfId="141" priority="198" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="217" stopIfTrue="1">
       <formula>BQ56&lt;&gt;BQ55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ57:BR57">
-    <cfRule type="expression" dxfId="140" priority="197" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="216" stopIfTrue="1">
       <formula>BQ57&lt;&gt;BQ56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ58:BR58">
-    <cfRule type="expression" dxfId="139" priority="196" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="215" stopIfTrue="1">
       <formula>BQ58&lt;&gt;BQ57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ59:BR65">
-    <cfRule type="expression" dxfId="138" priority="195" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="214" stopIfTrue="1">
       <formula>BQ59&lt;&gt;BQ58</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ66:BR66">
-    <cfRule type="expression" dxfId="137" priority="194" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="213" stopIfTrue="1">
       <formula>BQ66&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ67:BR67">
-    <cfRule type="expression" dxfId="136" priority="193" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="212" stopIfTrue="1">
       <formula>BQ67&lt;&gt;BQ66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ68:BR68">
-    <cfRule type="expression" dxfId="135" priority="192" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="211" stopIfTrue="1">
       <formula>BQ68&lt;&gt;BQ67</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ69:BR69">
-    <cfRule type="expression" dxfId="134" priority="191" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="210" stopIfTrue="1">
       <formula>BQ69&lt;&gt;BQ68</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ70:BR76">
-    <cfRule type="expression" dxfId="133" priority="190" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="209" stopIfTrue="1">
       <formula>BQ70&lt;&gt;BQ69</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ77:BR77">
-    <cfRule type="expression" dxfId="132" priority="189" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="208" stopIfTrue="1">
       <formula>BQ77&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ78:BR78">
-    <cfRule type="expression" dxfId="131" priority="188" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="207" stopIfTrue="1">
       <formula>BQ78&lt;&gt;BQ77</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ79:BR79">
-    <cfRule type="expression" dxfId="130" priority="187" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="206" stopIfTrue="1">
       <formula>BQ79&lt;&gt;BQ78</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ80:BR80">
-    <cfRule type="expression" dxfId="129" priority="186" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="205" stopIfTrue="1">
       <formula>BQ80&lt;&gt;BQ79</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ81:BR87">
-    <cfRule type="expression" dxfId="128" priority="185" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="204" stopIfTrue="1">
       <formula>BQ81&lt;&gt;BQ80</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ88:BR88">
-    <cfRule type="expression" dxfId="127" priority="184" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="203" stopIfTrue="1">
       <formula>BQ88&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ89:BR89">
-    <cfRule type="expression" dxfId="126" priority="183" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="202" stopIfTrue="1">
       <formula>BQ89&lt;&gt;BQ88</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ90:BR90">
-    <cfRule type="expression" dxfId="125" priority="182" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="201" stopIfTrue="1">
       <formula>BQ90&lt;&gt;BQ89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ91:BR91">
-    <cfRule type="expression" dxfId="124" priority="181" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="200" stopIfTrue="1">
       <formula>BQ91&lt;&gt;BQ90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ92:BR98">
-    <cfRule type="expression" dxfId="123" priority="180" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="199" stopIfTrue="1">
       <formula>BQ92&lt;&gt;BQ91</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ99:BR99">
-    <cfRule type="expression" dxfId="122" priority="179" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="198" stopIfTrue="1">
       <formula>BQ99&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ100:BR100">
-    <cfRule type="expression" dxfId="121" priority="178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="197" stopIfTrue="1">
       <formula>BQ100&lt;&gt;BQ99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ101:BR101">
-    <cfRule type="expression" dxfId="120" priority="177" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="196" stopIfTrue="1">
       <formula>BQ101&lt;&gt;BQ100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ102:BR102">
-    <cfRule type="expression" dxfId="119" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="195" stopIfTrue="1">
       <formula>BQ102&lt;&gt;BQ101</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BQ103:BR109">
-    <cfRule type="expression" dxfId="118" priority="175" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="194" stopIfTrue="1">
       <formula>BQ103&lt;&gt;BQ102</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z22:Z32">
-    <cfRule type="cellIs" dxfId="117" priority="161" operator="lessThan">
+    <cfRule type="cellIs" dxfId="136" priority="180" operator="lessThan">
       <formula>Y22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA22:AA32">
-    <cfRule type="cellIs" dxfId="116" priority="159" operator="lessThan">
+    <cfRule type="cellIs" dxfId="135" priority="178" operator="lessThan">
       <formula>Z22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z33:Z43">
-    <cfRule type="cellIs" dxfId="115" priority="157" operator="lessThan">
+    <cfRule type="cellIs" dxfId="134" priority="176" operator="lessThan">
       <formula>Y33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA33:AA43">
-    <cfRule type="cellIs" dxfId="114" priority="155" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="174" operator="lessThan">
       <formula>Z33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44:Z54">
-    <cfRule type="cellIs" dxfId="113" priority="153" operator="lessThan">
+    <cfRule type="cellIs" dxfId="132" priority="172" operator="lessThan">
       <formula>Y44</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AA54">
-    <cfRule type="cellIs" dxfId="112" priority="151" operator="lessThan">
+    <cfRule type="cellIs" dxfId="131" priority="170" operator="lessThan">
       <formula>Z44</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z55:Z65">
-    <cfRule type="cellIs" dxfId="111" priority="149" operator="lessThan">
+    <cfRule type="cellIs" dxfId="130" priority="168" operator="lessThan">
       <formula>Y55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA55:AA65">
-    <cfRule type="cellIs" dxfId="110" priority="147" operator="lessThan">
+    <cfRule type="cellIs" dxfId="129" priority="166" operator="lessThan">
       <formula>Z55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z66:Z76">
-    <cfRule type="cellIs" dxfId="109" priority="145" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="164" operator="lessThan">
       <formula>Y66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA66:AA76">
-    <cfRule type="cellIs" dxfId="108" priority="143" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="162" operator="lessThan">
       <formula>Z66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z77:Z87">
-    <cfRule type="cellIs" dxfId="107" priority="141" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="160" operator="lessThan">
       <formula>Y77</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA77:AA87">
-    <cfRule type="cellIs" dxfId="106" priority="139" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="158" operator="lessThan">
       <formula>Z77</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z88:Z98">
-    <cfRule type="cellIs" dxfId="105" priority="137" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="156" operator="lessThan">
       <formula>Y88</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA88:AA98">
-    <cfRule type="cellIs" dxfId="104" priority="135" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="154" operator="lessThan">
       <formula>Z88</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z99:Z109">
-    <cfRule type="cellIs" dxfId="103" priority="133" operator="lessThan">
+  <conditionalFormatting sqref="Z99:Z120">
+    <cfRule type="cellIs" dxfId="122" priority="152" operator="lessThan">
       <formula>Y99</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA99:AA109">
-    <cfRule type="cellIs" dxfId="102" priority="131" operator="lessThan">
+  <conditionalFormatting sqref="AA99:AA120">
+    <cfRule type="cellIs" dxfId="121" priority="150" operator="lessThan">
       <formula>Z99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="cellIs" dxfId="101" priority="125" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="144" operator="lessThan">
       <formula>AA2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB2">
-    <cfRule type="expression" dxfId="100" priority="124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="143" stopIfTrue="1">
       <formula>AB2&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB11">
-    <cfRule type="cellIs" dxfId="99" priority="123" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="142" operator="lessThan">
       <formula>AA11</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB11">
-    <cfRule type="expression" dxfId="98" priority="122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="141" stopIfTrue="1">
       <formula>AB11&lt;&gt;AB10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3">
-    <cfRule type="cellIs" dxfId="97" priority="121" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="140" operator="lessThan">
       <formula>AA3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB3">
-    <cfRule type="expression" dxfId="96" priority="120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="139" stopIfTrue="1">
       <formula>AB3&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB6">
-    <cfRule type="cellIs" dxfId="95" priority="119" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="138" operator="lessThan">
       <formula>AA6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB6">
-    <cfRule type="expression" dxfId="94" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="137" stopIfTrue="1">
       <formula>AB6&lt;&gt;AB5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB9">
-    <cfRule type="cellIs" dxfId="93" priority="117" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="136" operator="lessThan">
       <formula>AA9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB9">
-    <cfRule type="expression" dxfId="92" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="135" stopIfTrue="1">
       <formula>AB9&lt;&gt;AB8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB12">
-    <cfRule type="cellIs" dxfId="91" priority="115" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="134" operator="lessThan">
       <formula>AA12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB12">
-    <cfRule type="expression" dxfId="90" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="133" stopIfTrue="1">
       <formula>AB12&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB14">
-    <cfRule type="cellIs" dxfId="89" priority="111" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="130" operator="lessThan">
       <formula>AA14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB14">
-    <cfRule type="expression" dxfId="88" priority="110" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="129" stopIfTrue="1">
       <formula>AB14&lt;&gt;AB13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB17">
-    <cfRule type="cellIs" dxfId="87" priority="109" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="128" operator="lessThan">
       <formula>AA17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB17">
-    <cfRule type="expression" dxfId="86" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="127" stopIfTrue="1">
       <formula>AB17&lt;&gt;AB16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB20">
-    <cfRule type="cellIs" dxfId="85" priority="107" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="126" operator="lessThan">
       <formula>AA20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB20">
-    <cfRule type="expression" dxfId="84" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="125" stopIfTrue="1">
       <formula>AB20&lt;&gt;AB19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB22">
-    <cfRule type="cellIs" dxfId="83" priority="105" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="124" operator="lessThan">
       <formula>AA22</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB22">
-    <cfRule type="expression" dxfId="82" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="123" stopIfTrue="1">
       <formula>AB22&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB32">
-    <cfRule type="cellIs" dxfId="81" priority="103" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="122" operator="lessThan">
       <formula>AA32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB32">
-    <cfRule type="expression" dxfId="80" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="121" stopIfTrue="1">
       <formula>AB32&lt;&gt;AB31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB24">
-    <cfRule type="cellIs" dxfId="79" priority="101" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="120" operator="lessThan">
       <formula>AA24</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB24">
-    <cfRule type="expression" dxfId="78" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="119" stopIfTrue="1">
       <formula>AB24&lt;&gt;AB23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB27">
-    <cfRule type="cellIs" dxfId="77" priority="99" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="118" operator="lessThan">
       <formula>AA27</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB27">
-    <cfRule type="expression" dxfId="76" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="117" stopIfTrue="1">
       <formula>AB27&lt;&gt;AB26</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB30">
-    <cfRule type="cellIs" dxfId="75" priority="97" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="116" operator="lessThan">
       <formula>AA30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB30">
-    <cfRule type="expression" dxfId="74" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="115" stopIfTrue="1">
       <formula>AB30&lt;&gt;AB29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB44">
-    <cfRule type="cellIs" dxfId="73" priority="95" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="114" operator="lessThan">
       <formula>AA44</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB44">
-    <cfRule type="expression" dxfId="72" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="113" stopIfTrue="1">
       <formula>AB44&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB54">
-    <cfRule type="cellIs" dxfId="71" priority="93" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="112" operator="lessThan">
       <formula>AA54</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB54">
-    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="111" stopIfTrue="1">
       <formula>AB54&lt;&gt;AB53</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB46">
-    <cfRule type="cellIs" dxfId="69" priority="91" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="110" operator="lessThan">
       <formula>AA46</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB46">
-    <cfRule type="expression" dxfId="68" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="109" stopIfTrue="1">
       <formula>AB46&lt;&gt;AB45</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB49">
-    <cfRule type="cellIs" dxfId="67" priority="89" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="108" operator="lessThan">
       <formula>AA49</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB49">
-    <cfRule type="expression" dxfId="66" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="107" stopIfTrue="1">
       <formula>AB49&lt;&gt;AB48</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB52">
-    <cfRule type="cellIs" dxfId="65" priority="87" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="106" operator="lessThan">
       <formula>AA52</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB52">
-    <cfRule type="expression" dxfId="64" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="105" stopIfTrue="1">
       <formula>AB52&lt;&gt;AB51</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB21">
-    <cfRule type="cellIs" dxfId="63" priority="75" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="94" operator="lessThan">
       <formula>AA21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB21">
-    <cfRule type="expression" dxfId="62" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="93" stopIfTrue="1">
       <formula>AB21&lt;&gt;AB20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB33">
-    <cfRule type="cellIs" dxfId="61" priority="73" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="92" operator="lessThan">
       <formula>AA33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB33">
-    <cfRule type="expression" dxfId="60" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="91" stopIfTrue="1">
       <formula>AB33&lt;&gt;AB32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB43">
-    <cfRule type="cellIs" dxfId="59" priority="71" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="90" operator="lessThan">
       <formula>AA43</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB43">
-    <cfRule type="expression" dxfId="58" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="89" stopIfTrue="1">
       <formula>AB43&lt;&gt;AB42</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB35">
-    <cfRule type="cellIs" dxfId="57" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="88" operator="lessThan">
       <formula>AA35</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB35">
-    <cfRule type="expression" dxfId="56" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="87" stopIfTrue="1">
       <formula>AB35&lt;&gt;AB34</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB38">
-    <cfRule type="cellIs" dxfId="55" priority="67" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="86" operator="lessThan">
       <formula>AA38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB38">
-    <cfRule type="expression" dxfId="54" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="85" stopIfTrue="1">
       <formula>AB38&lt;&gt;AB37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB41">
-    <cfRule type="cellIs" dxfId="53" priority="65" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="84" operator="lessThan">
       <formula>AA41</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB41">
-    <cfRule type="expression" dxfId="52" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="83" stopIfTrue="1">
       <formula>AB41&lt;&gt;AB40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB55">
-    <cfRule type="cellIs" dxfId="51" priority="63" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="82" operator="lessThan">
       <formula>AA55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB55">
-    <cfRule type="expression" dxfId="50" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="81" stopIfTrue="1">
       <formula>AB55&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB65">
-    <cfRule type="cellIs" dxfId="49" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="80" operator="lessThan">
       <formula>AA65</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB65">
-    <cfRule type="expression" dxfId="48" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="79" stopIfTrue="1">
       <formula>AB65&lt;&gt;AB64</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB57">
-    <cfRule type="cellIs" dxfId="47" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="78" operator="lessThan">
       <formula>AA57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB57">
-    <cfRule type="expression" dxfId="46" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="77" stopIfTrue="1">
       <formula>AB57&lt;&gt;AB56</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB60">
-    <cfRule type="cellIs" dxfId="45" priority="57" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="76" operator="lessThan">
       <formula>AA60</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB60">
-    <cfRule type="expression" dxfId="44" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="75" stopIfTrue="1">
       <formula>AB60&lt;&gt;AB59</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB63">
-    <cfRule type="cellIs" dxfId="43" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="74" operator="lessThan">
       <formula>AA63</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB63">
-    <cfRule type="expression" dxfId="42" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="73" stopIfTrue="1">
       <formula>AB63&lt;&gt;AB62</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB77">
-    <cfRule type="cellIs" dxfId="41" priority="53" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="72" operator="lessThan">
       <formula>AA77</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB77">
-    <cfRule type="expression" dxfId="40" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="71" stopIfTrue="1">
       <formula>AB77&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB87">
-    <cfRule type="cellIs" dxfId="39" priority="51" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="70" operator="lessThan">
       <formula>AA87</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB87">
-    <cfRule type="expression" dxfId="38" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="69" stopIfTrue="1">
       <formula>AB87&lt;&gt;AB86</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB79">
-    <cfRule type="cellIs" dxfId="37" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="68" operator="lessThan">
       <formula>AA79</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB79">
-    <cfRule type="expression" dxfId="36" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="67" stopIfTrue="1">
       <formula>AB79&lt;&gt;AB78</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB82">
-    <cfRule type="cellIs" dxfId="35" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="66" operator="lessThan">
       <formula>AA82</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB82">
-    <cfRule type="expression" dxfId="34" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="65" stopIfTrue="1">
       <formula>AB82&lt;&gt;AB81</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB85">
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="64" operator="lessThan">
       <formula>AA85</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB85">
-    <cfRule type="expression" dxfId="32" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="63" stopIfTrue="1">
       <formula>AB85&lt;&gt;AB84</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB88">
-    <cfRule type="cellIs" dxfId="31" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="62" operator="lessThan">
       <formula>AA88</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB88">
-    <cfRule type="expression" dxfId="30" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="61" stopIfTrue="1">
       <formula>AB88&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB98">
-    <cfRule type="cellIs" dxfId="29" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="60" operator="lessThan">
       <formula>AA98</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB98">
-    <cfRule type="expression" dxfId="28" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="59" stopIfTrue="1">
       <formula>AB98&lt;&gt;AB97</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB90">
-    <cfRule type="cellIs" dxfId="27" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="58" operator="lessThan">
       <formula>AA90</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB90">
-    <cfRule type="expression" dxfId="26" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="57" stopIfTrue="1">
       <formula>AB90&lt;&gt;AB89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB93">
-    <cfRule type="cellIs" dxfId="25" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="56" operator="lessThan">
       <formula>AA93</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB93">
-    <cfRule type="expression" dxfId="24" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="55" stopIfTrue="1">
       <formula>AB93&lt;&gt;AB92</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB96">
-    <cfRule type="cellIs" dxfId="23" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="54" operator="lessThan">
       <formula>AA96</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB96">
-    <cfRule type="expression" dxfId="22" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="53" stopIfTrue="1">
       <formula>AB96&lt;&gt;AB95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB66">
-    <cfRule type="cellIs" dxfId="21" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="52" operator="lessThan">
       <formula>AA66</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB66">
-    <cfRule type="expression" dxfId="20" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="51" stopIfTrue="1">
       <formula>AB66&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB76">
-    <cfRule type="cellIs" dxfId="19" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="50" operator="lessThan">
       <formula>AA76</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB76">
-    <cfRule type="expression" dxfId="18" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="49" stopIfTrue="1">
       <formula>AB76&lt;&gt;AB75</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB68">
-    <cfRule type="cellIs" dxfId="17" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="lessThan">
       <formula>AA68</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB68">
-    <cfRule type="expression" dxfId="16" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="47" stopIfTrue="1">
       <formula>AB68&lt;&gt;AB67</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB71">
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="46" operator="lessThan">
       <formula>AA71</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB71">
-    <cfRule type="expression" dxfId="14" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="45" stopIfTrue="1">
       <formula>AB71&lt;&gt;AB70</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB74">
-    <cfRule type="cellIs" dxfId="13" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="44" operator="lessThan">
       <formula>AA74</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB74">
-    <cfRule type="expression" dxfId="12" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="43" stopIfTrue="1">
       <formula>AB74&lt;&gt;AB73</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB99">
-    <cfRule type="cellIs" dxfId="11" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="42" operator="lessThan">
       <formula>AA99</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB99">
-    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="41" stopIfTrue="1">
       <formula>AB99&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB109">
-    <cfRule type="cellIs" dxfId="9" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="40" operator="lessThan">
       <formula>AA109</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB109">
-    <cfRule type="expression" dxfId="8" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="39" stopIfTrue="1">
       <formula>AB109&lt;&gt;AB108</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB101">
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="38" operator="lessThan">
       <formula>AA101</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB101">
-    <cfRule type="expression" dxfId="6" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="37" stopIfTrue="1">
       <formula>AB101&lt;&gt;AB100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB104">
-    <cfRule type="cellIs" dxfId="5" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="36" operator="lessThan">
       <formula>AA104</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB104">
-    <cfRule type="expression" dxfId="4" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="35" stopIfTrue="1">
       <formula>AB104&lt;&gt;AB103</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB107">
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="34" operator="lessThan">
       <formula>AA107</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB107">
-    <cfRule type="expression" dxfId="2" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="33" stopIfTrue="1">
       <formula>AB107&lt;&gt;AB106</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y109">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="Y2:Y120">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="lessThan">
       <formula>$X$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC2:AC109">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+  <conditionalFormatting sqref="AC2:AC108">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="lessThan">
       <formula>X2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z111:AA120">
+    <cfRule type="expression" dxfId="18" priority="19" stopIfTrue="1">
+      <formula>Z111&lt;&gt;Z110</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z110:AA110">
+    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+      <formula>Z110&lt;&gt;#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ110:BR110">
+    <cfRule type="expression" dxfId="16" priority="17" stopIfTrue="1">
+      <formula>BQ110&lt;&gt;#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ111:BR111">
+    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+      <formula>BQ111&lt;&gt;BQ110</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ112:BR112">
+    <cfRule type="expression" dxfId="14" priority="15" stopIfTrue="1">
+      <formula>BQ112&lt;&gt;BQ111</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ113:BR113">
+    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+      <formula>BQ113&lt;&gt;BQ112</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ114:BR120">
+    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
+      <formula>BQ114&lt;&gt;BQ113</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB110">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
+      <formula>AA110</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB110">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
+      <formula>AB110&lt;&gt;#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB120">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
+      <formula>AA120</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB120">
+    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+      <formula>AB120&lt;&gt;AB119</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB112">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+      <formula>AA112</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB112">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+      <formula>AB112&lt;&gt;AB111</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB115">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+      <formula>AA115</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB115">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+      <formula>AB115&lt;&gt;AB114</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB118">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>AA118</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB118">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>AB118&lt;&gt;AB117</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC109:AC120">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>AB109</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC109:AC120">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>$X$2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>